<commit_message>
completed ages ago just moving to github
</commit_message>
<xml_diff>
--- a/inductive reactance/experiment1.xlsx
+++ b/inductive reactance/experiment1.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\GitHub\AH-Physics-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\GitHub\AH-Physics-Project\inductive reactance\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D4F054-5086-4B66-B41A-E013506C308F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>avg</t>
   </si>
@@ -98,6 +99,18 @@
   <si>
     <t>1/F</t>
   </si>
+  <si>
+    <t>gradient</t>
+  </si>
+  <si>
+    <t>∆gradient</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>∆intercept</t>
+  </si>
 </sst>
 </file>
 
@@ -138,11 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2602,10 +2616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2617,7 +2631,7 @@
     <col min="5" max="5" width="12.5546875" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
     <col min="16" max="16" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3162,13 +3176,16 @@
         <v>1.1509999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C21">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C19">
         <f>(5/(2*PI()*D22))</f>
         <v>0.32711531549582401</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
       <c r="D22">
         <f t="array" ref="D22:E23">LINEST(R3:R9,B3:B9,TRUE,TRUE)</f>
         <v>2.432703935776543</v>
@@ -3176,17 +3193,55 @@
       <c r="E22">
         <v>-7.5253229128757694E-5</v>
       </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D23">
         <v>4.4827398286020233E-2</v>
       </c>
       <c r="E23">
         <v>1.8241036805583528E-5</v>
       </c>
+      <c r="F23" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D25">
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25">
+        <v>2.432703935776543</v>
+      </c>
+      <c r="J25">
+        <f>-7.52532*10^-5</f>
+        <v>-7.5253200000000007E-5</v>
+      </c>
+      <c r="K25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26">
+        <v>4.4827398286020233E-2</v>
+      </c>
+      <c r="J26">
+        <v>1.8241036805583528E-5</v>
+      </c>
+      <c r="K26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D27">
         <f>(D23/D22)*100</f>
         <v>1.8426984733639973</v>
       </c>

</xml_diff>